<commit_message>
include project ID and indicator (section code only for now)
</commit_message>
<xml_diff>
--- a/app/data-projects.xlsx
+++ b/app/data-projects.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t xml:space="preserve">Improving MRV Capabilities on Carbon Accounting to Support REDD+ Jurisdictional Programs in Brazilian Amazon States</t>
   </si>
   <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e1650ae0-a39c-11e6-a738-31c333ef0e28</t>
+  </si>
+  <si>
     <t xml:space="preserve">subcontractor</t>
   </si>
   <si>
@@ -64,9 +70,24 @@
     <t xml:space="preserve">BRA-AP</t>
   </si>
   <si>
+    <t xml:space="preserve">indicators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Strengthening State-Level Capacities to Estimate, Analyze and Report Emissions From the Forest Sector Aligned With Mexico’s National System for REDD+ MRV</t>
   </si>
   <si>
+    <t xml:space="preserve">e75a9dc0-a39c-11e6-a738-31c333ef0e28</t>
+  </si>
+  <si>
     <t xml:space="preserve">ECOSUR</t>
   </si>
   <si>
@@ -104,6 +125,12 @@
   </si>
   <si>
     <t xml:space="preserve">MEX-ROO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.b</t>
   </si>
 </sst>
 </file>
@@ -179,12 +206,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,18 +236,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -229,7 +258,7 @@
       <c r="B2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -266,52 +295,58 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="0"/>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="1" t="s">
-        <v>19</v>
+      <c r="C15" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,51 +354,92 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>5</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>5</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include references to indicators
</commit_message>
<xml_diff>
--- a/app/data-projects.xlsx
+++ b/app/data-projects.xlsx
@@ -73,13 +73,13 @@
     <t xml:space="preserve">indicators</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.6.c</t>
+    <t xml:space="preserve">1.1 a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4 a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6 c</t>
   </si>
   <si>
     <t xml:space="preserve">Strengthening State-Level Capacities to Estimate, Analyze and Report Emissions From the Forest Sector Aligned With Mexico’s National System for REDD+ MRV</t>
@@ -127,10 +127,10 @@
     <t xml:space="preserve">MEX-ROO</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.b</t>
+    <t xml:space="preserve">1.1 c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2 b</t>
   </si>
 </sst>
 </file>
@@ -239,13 +239,15 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>